<commit_message>
filter and sort feature
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/testdata.xlsx
+++ b/src/test/resources/datatest/testdata.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fam2536/Desktop/Working/PayActive/Automation/automation-payActive/src/test/resources/datatest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fam2536/Desktop/Working/PayActive/AutomationTest/automation-payActive/src/test/resources/datatest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CA40E7-A7A9-B840-B0D1-ED0ADD956C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0542D341-E5FB-3140-8675-E37FB02BB582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30940" windowHeight="16780" xr2:uid="{087FA7D4-EF6F-413D-ABC6-FDC0D1BECD89}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20420" activeTab="1" xr2:uid="{087FA7D4-EF6F-413D-ABC6-FDC0D1BECD89}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Customer" sheetId="2" r:id="rId2"/>
+    <sheet name="Filter" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,18 +26,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>Employer_Darden1</t>
-  </si>
-  <si>
-    <t>Tester567892</t>
-  </si>
-  <si>
     <t>USERNAME</t>
+  </si>
+  <si>
+    <t>FPTTeam</t>
+  </si>
+  <si>
+    <t>123@a123</t>
+  </si>
+  <si>
+    <t>EmployeeName</t>
+  </si>
+  <si>
+    <t>EmployeeId</t>
+  </si>
+  <si>
+    <t>Departments</t>
+  </si>
+  <si>
+    <t>CardStatus</t>
+  </si>
+  <si>
+    <t>CardType</t>
+  </si>
+  <si>
+    <t>mmaa</t>
+  </si>
+  <si>
+    <t>A4352</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Activated</t>
+  </si>
+  <si>
+    <t>Instant Issue</t>
   </si>
 </sst>
 </file>
@@ -402,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72AD5D9-45AB-4B7A-B8DD-0D8E68C91E98}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -414,7 +444,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -422,15 +452,16 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="admin@example.com" xr:uid="{51DB2703-F548-4893-9C4E-63DC652B5850}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{58A1E20F-4C00-8148-BBE8-A05052B008F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -438,14 +469,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7D98F3-2EDE-4E23-83ED-4B5338E51797}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Load History and view account info
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/testdata.xlsx
+++ b/src/test/resources/datatest/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fam2536/Desktop/Working/PayActive/AutomationTest/automation-payActive/src/test/resources/datatest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0542D341-E5FB-3140-8675-E37FB02BB582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD85B-FBA5-3445-AD4E-5073CBC6E795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20420" activeTab="1" xr2:uid="{087FA7D4-EF6F-413D-ABC6-FDC0D1BECD89}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Filter" sheetId="2" r:id="rId2"/>
+    <sheet name="CardHolderFilter" sheetId="2" r:id="rId2"/>
+    <sheet name="LoadHistoryFilter" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>PASSWORD</t>
   </si>
@@ -46,9 +47,6 @@
     <t>EmployeeId</t>
   </si>
   <si>
-    <t>Departments</t>
-  </si>
-  <si>
     <t>CardStatus</t>
   </si>
   <si>
@@ -68,6 +66,15 @@
   </si>
   <si>
     <t>Instant Issue</t>
+  </si>
+  <si>
+    <t>escalation</t>
+  </si>
+  <si>
+    <t>Last4Digits</t>
+  </si>
+  <si>
+    <t>Department</t>
   </si>
 </sst>
 </file>
@@ -472,7 +479,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,30 +499,80 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5726E21-F989-544F-81CD-4576D0C0C399}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>455545</v>
+      </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>3802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>